<commit_message>
added some images for my Insomnia methods
</commit_message>
<xml_diff>
--- a/REST-API-Specs.xlsx
+++ b/REST-API-Specs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulinehawker/Desktop/DRF_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B730BDF-C8D2-BA42-BEE3-3BE34D1AD428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786BC49F-051A-7B4B-A1F7-AD93AD49C6A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14060" yWindow="500" windowWidth="14740" windowHeight="16220" xr2:uid="{BEFD6ACC-63D0-4846-84C8-8A0A9F43732C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
   <si>
     <t>Rest API Specifications</t>
   </si>
@@ -112,12 +112,6 @@
   <si>
     <t>Must be logged in.
 Must be the project owner</t>
-  </si>
-  <si>
-    <t>knowmads/</t>
-  </si>
-  <si>
-    <t>Page not found</t>
   </si>
 </sst>
 </file>
@@ -492,7 +486,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="35" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -678,19 +672,11 @@
     </row>
     <row r="10" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
-      <c r="B10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>26</v>
-      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="3">
-        <v>404</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>

</xml_diff>

<commit_message>
updated my readme for the project
</commit_message>
<xml_diff>
--- a/REST-API-Specs.xlsx
+++ b/REST-API-Specs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulinehawker/Desktop/DRF_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786BC49F-051A-7B4B-A1F7-AD93AD49C6A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12AB6500-0686-6242-9F80-6347AF2F8773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14060" yWindow="500" windowWidth="14740" windowHeight="16220" xr2:uid="{BEFD6ACC-63D0-4846-84C8-8A0A9F43732C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="13640" windowHeight="16220" xr2:uid="{BEFD6ACC-63D0-4846-84C8-8A0A9F43732C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="38">
   <si>
     <t>Rest API Specifications</t>
   </si>
@@ -90,12 +90,6 @@
   </si>
   <si>
     <t>Updates the project with ID of '1'</t>
-  </si>
-  <si>
-    <t>Creates a new pledge.</t>
-  </si>
-  <si>
-    <t>Get the pledge with ID of '1'</t>
   </si>
   <si>
     <t>Deletes the pledge with ID of '1'</t>
@@ -112,6 +106,51 @@
   <si>
     <t>Must be logged in.
 Must be the project owner</t>
+  </si>
+  <si>
+    <t>Deletes the project with ID of '1'</t>
+  </si>
+  <si>
+    <t>/pledges/1</t>
+  </si>
+  <si>
+    <t>Pledge object.</t>
+  </si>
+  <si>
+    <t>Returns all pledges.</t>
+  </si>
+  <si>
+    <t>Create a new pledge.</t>
+  </si>
+  <si>
+    <t>Returns the pledge with ID of '1'</t>
+  </si>
+  <si>
+    <t>Updates the pledge with ID of '1'</t>
+  </si>
+  <si>
+    <t>/users/</t>
+  </si>
+  <si>
+    <t>/users/1</t>
+  </si>
+  <si>
+    <t>User object.</t>
+  </si>
+  <si>
+    <t>Returns all users.</t>
+  </si>
+  <si>
+    <t>Create a new user.</t>
+  </si>
+  <si>
+    <t>Returns the user with ID of '1'</t>
+  </si>
+  <si>
+    <t>Updates the user with ID of '1'</t>
+  </si>
+  <si>
+    <t>Deletes the user with ID of '1'</t>
   </si>
 </sst>
 </file>
@@ -483,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0ACD445-AAE9-0C4B-948E-DAA82015D22C}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="35" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -541,13 +580,13 @@
         <v>14</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E3" s="3">
         <v>200</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
@@ -561,13 +600,13 @@
         <v>15</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E4" s="3">
         <v>201</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
@@ -581,13 +620,13 @@
         <v>16</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E5" s="3">
         <v>200</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
@@ -601,33 +640,33 @@
         <v>17</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="3">
+        <v>200</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="E6" s="3">
-        <v>200</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="3">
+        <v>200</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="E7" s="3">
-        <v>201</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
@@ -638,93 +677,197 @@
         <v>13</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E8" s="3">
         <v>200</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="3">
+        <v>201</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="3">
-        <v>200</v>
-      </c>
-      <c r="F9" s="3" t="s">
+    </row>
+    <row r="10" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="3">
+        <v>200</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="11" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
+      <c r="A11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="3">
+        <v>200</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
+      <c r="A12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="3">
+        <v>200</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
+      <c r="A13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="3">
+        <v>200</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="14" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
+      <c r="A14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="3">
+        <v>201</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="15" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
+      <c r="A15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="3">
+        <v>200</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
+      <c r="A16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="3">
+        <v>200</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="3">
+        <v>200</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>